<commit_message>
Normalize all the line endings
</commit_message>
<xml_diff>
--- a/src/main/resources/static/resources/TeamSheet.xlsx
+++ b/src/main/resources/static/resources/TeamSheet.xlsx
@@ -1,19 +1,3 @@
-
-<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-  </sheets>
-  <calcPr calcId="145621"/>
-</workbook>
-</file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
@@ -751,291 +735,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
@@ -1562,28 +1261,4 @@
     </mc:Choice>
   </mc:AlternateContent>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>